<commit_message>
added Usability Testkonzept to Readme
</commit_message>
<xml_diff>
--- a/Kommentare/Usability-Testkonzept/AB-Tests.xlsx
+++ b/Kommentare/Usability-Testkonzept/AB-Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57a0ea7baa69ea17/Studium/Semester 3/Softwareergonomie und grafische Benutzeroberflächen/Projektv1/Fitnesso/Kommentare/Usability-Testkonzept/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_AD4DB114E441178AC67DF4563693CBF2693EDF1A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6957E9C8-E7BF-4D3F-A2DA-EF991E322B1E}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="11_AD4DB114E441178AC67DF4563693CBF2693EDF1A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C445831E-1A03-4503-81EF-7297CE023385}"/>
   <bookViews>
     <workbookView xWindow="8940" yWindow="7425" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>A (Sekunden)</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>AVG B:</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -106,7 +109,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C921F62-9B50-435D-A8F4-2CB9E948DC20}" name="Tabelle1" displayName="Tabelle1" ref="A1:B11" totalsRowShown="0">
   <autoFilter ref="A1:B11" xr:uid="{407C1613-2BA5-4FBF-AAA9-2582B0EA289E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6A173E25-A08B-4B91-A114-C0821BB3B2B1}" name="A (Sekunden)"/>
+    <tableColumn id="1" xr3:uid="{6A173E25-A08B-4B91-A114-C0821BB3B2B1}" name="c"/>
     <tableColumn id="2" xr3:uid="{98762912-205C-4FAA-A1B5-2BFA4ED84B46}" name="B (Sekunden)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -401,7 +404,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +415,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -508,7 +511,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>AVERAGE(Tabelle1[A (Sekunden)])</f>
+        <f>AVERAGE(Tabelle1[c])</f>
         <v>51.3</v>
       </c>
       <c r="B15">
@@ -518,8 +521,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>